<commit_message>
Dashboard Outline V6 ( Complete )
fix date to be 10/05/2020 ka
</commit_message>
<xml_diff>
--- a/FN312_Dashboard_Outline_V6.xlsx
+++ b/FN312_Dashboard_Outline_V6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\JaJa\FN312\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B65DEF-72D8-409C-BD19-489E363F6107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B230DE-23BE-4500-8518-206F4C41C00D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -2303,83 +2303,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2406,13 +2333,16 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2433,7 +2363,82 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2454,7 +2459,46 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2475,7 +2519,79 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2493,7 +2609,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -2550,73 +2666,61 @@
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -2643,7 +2747,166 @@
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
@@ -2668,6 +2931,25 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -2799,343 +3081,13 @@
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -3187,6 +3139,54 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8961,42 +8961,42 @@
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Transaction Date"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Transactions"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Cancel Reason"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Amount" dataDxfId="156"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Execution_Price" dataDxfId="155"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Month_order" dataDxfId="154">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Amount" dataDxfId="254"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Execution_Price" dataDxfId="253"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Month_order" dataDxfId="252">
       <calculatedColumnFormula>VALUE(LEFT(tbl_transaction[[#This Row],[Order Date]],FIND("/",tbl_transaction[[#This Row],[Order Date]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Date_order" dataDxfId="153">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Date_order" dataDxfId="251">
       <calculatedColumnFormula>MID(tbl_transaction[[#This Row],[Order Date]], FIND("/",tbl_transaction[[#This Row],[Order Date]])+1, FIND("/",tbl_transaction[[#This Row],[Order Date]], FIND("/",tbl_transaction[[#This Row],[Order Date]])+1)-FIND("/",tbl_transaction[[#This Row],[Order Date]])-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Year_order" dataDxfId="152">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Year_order" dataDxfId="250">
       <calculatedColumnFormula>MID(tbl_transaction[[#This Row],[Order Date]], FIND("/",tbl_transaction[[#This Row],[Order Date]], FIND("/", tbl_transaction[[#This Row],[Order Date]])+1)+1, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Month_Transact" dataDxfId="151">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Month_Transact" dataDxfId="249">
       <calculatedColumnFormula>VALUE(LEFT(tbl_transaction[[#This Row],[Transaction Date]],FIND("/",tbl_transaction[[#This Row],[Transaction Date]])-1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Date_Transact" dataDxfId="150">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Date_Transact" dataDxfId="248">
       <calculatedColumnFormula>MID(tbl_transaction[[#This Row],[Transaction Date]], FIND("/",tbl_transaction[[#This Row],[Transaction Date]])+1, FIND("/",tbl_transaction[[#This Row],[Transaction Date]], FIND("/",tbl_transaction[[#This Row],[Transaction Date]])+1)-FIND("/",tbl_transaction[[#This Row],[Transaction Date]])-1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Year_Transact" dataDxfId="149">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Year_Transact" dataDxfId="247">
       <calculatedColumnFormula>MID(tbl_transaction[[#This Row],[Transaction Date]], FIND("/",tbl_transaction[[#This Row],[Transaction Date]], FIND("/", tbl_transaction[[#This Row],[Transaction Date]])+1)+1, 2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Order_Date" dataDxfId="148">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Order_Date" dataDxfId="246">
       <calculatedColumnFormula>DATE(tbl_transaction[[#This Row],[Year_order]]+2000, tbl_transaction[[#This Row],[Month_order]], tbl_transaction[[#This Row],[Date_order]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Transaction_Date" dataDxfId="147">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Transaction_Date" dataDxfId="245">
       <calculatedColumnFormula>DATE(tbl_transaction[[#This Row],[Year_Transact]]+2000,tbl_transaction[[#This Row],[Month_Transact]],tbl_transaction[[#This Row],[Date_Transact]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Net_Cash_Change" totalsRowFunction="sum" dataDxfId="146" totalsRowDxfId="142">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Net_Cash_Change" totalsRowFunction="sum" dataDxfId="244" totalsRowDxfId="243">
       <calculatedColumnFormula>IF(tbl_transaction[[#This Row],[Transactions]]="Buy", -(tbl_transaction[[#This Row],[Amount]]*tbl_transaction[[#This Row],[Execution_Price]]), IF(tbl_transaction[[#This Row],[Transactions]]="Sell", tbl_transaction[[#This Row],[Amount]]*tbl_transaction[[#This Row],[Execution_Price]],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Net_Stock_Change" dataDxfId="145">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Net_Stock_Change" dataDxfId="242">
       <calculatedColumnFormula>IF(tbl_transaction[[#This Row],[Transactions]]="Buy", tbl_transaction[[#This Row],[Amount]]*tbl_transaction[[#This Row],[Execution_Price]], IF(tbl_transaction[[#This Row],[Transactions]]="Sell", -(tbl_transaction[[#This Row],[Amount]]*tbl_transaction[[#This Row],[Execution_Price]]), IF(tbl_transaction[[#This Row],[Transactions]]="Cover", -(tbl_transaction[[#This Row],[Amount]]*tbl_transaction[[#This Row],[Execution_Price]]), tbl_transaction[[#This Row],[Amount]]*tbl_transaction[[#This Row],[Execution_Price]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Net_Debt_Change" dataDxfId="144">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Net_Debt_Change" dataDxfId="241">
       <calculatedColumnFormula>IF(tbl_transaction[[#This Row],[Transactions]]="Short", tbl_transaction[[#This Row],[Amount]]*tbl_transaction[[#This Row],[Execution_Price]], IF(tbl_transaction[[#This Row],[Transactions]]="Cover", -(tbl_transaction[[#This Row],[Amount]]*tbl_transaction[[#This Row],[Execution_Price]]), 0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Stock Holding Change" totalsRowFunction="sum" dataDxfId="143" totalsRowDxfId="141">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Stock Holding Change" totalsRowFunction="sum" dataDxfId="240" totalsRowDxfId="239">
       <calculatedColumnFormula>IF(tbl_transaction[[#This Row],[Transactions]]="Buy", tbl_transaction[[#This Row],[Amount]], IF(tbl_transaction[[#This Row],[Transactions]]="Sell", -tbl_transaction[[#This Row],[Amount]], IF(tbl_transaction[[#This Row],[Transactions]]="Short", tbl_transaction[[#This Row],[Amount]], -tbl_transaction[[#This Row],[Amount]])))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9008,47 +9008,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="tbl_IBM" displayName="tbl_IBM" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Open" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="High" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Low" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Close" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Adj Close" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="124"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Open" dataDxfId="123"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="High" dataDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Low" dataDxfId="121"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Close" dataDxfId="120"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="Adj Close" dataDxfId="119"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0900-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="EMA" dataDxfId="74">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0900-000008000000}" name="EMA" dataDxfId="118">
       <calculatedColumnFormula>IF(tbl_IBM[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="RSI" dataDxfId="73">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0900-000009000000}" name="RSI" dataDxfId="117">
       <calculatedColumnFormula>IF(tbl_IBM[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_IBM[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="BB_Mean" dataDxfId="72">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0900-00000A000000}" name="BB_Mean" dataDxfId="116">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="BB_Upper" dataDxfId="71">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0900-00000B000000}" name="BB_Upper" dataDxfId="115">
       <calculatedColumnFormula>IF(tbl_IBM[[#This Row],[BB_Mean]]="", "", tbl_IBM[[#This Row],[BB_Mean]]+(BB_Width*tbl_IBM[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="BB_Lower" dataDxfId="70">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0900-00000C000000}" name="BB_Lower" dataDxfId="114">
       <calculatedColumnFormula>IF(tbl_IBM[[#This Row],[BB_Mean]]="", "", tbl_IBM[[#This Row],[BB_Mean]]-(BB_Width*tbl_IBM[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0900-00000D000000}" name="Move" dataDxfId="69">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0900-00000D000000}" name="Move" dataDxfId="113">
       <calculatedColumnFormula>IF(ROW(tbl_IBM[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="Upmove" dataDxfId="68">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0900-00000E000000}" name="Upmove" dataDxfId="112">
       <calculatedColumnFormula>MAX(tbl_IBM[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="Downmove" dataDxfId="67">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0900-00000F000000}" name="Downmove" dataDxfId="111">
       <calculatedColumnFormula>MAX(-tbl_IBM[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0900-000010000000}" name="Avg_Upmove" dataDxfId="66">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0900-000010000000}" name="Avg_Upmove" dataDxfId="110">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0900-000011000000}" name="Avg_Downmove" dataDxfId="65">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0900-000011000000}" name="Avg_Downmove" dataDxfId="109">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0900-000012000000}" name="RS" dataDxfId="64">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0900-000012000000}" name="RS" dataDxfId="108">
       <calculatedColumnFormula>IF(tbl_IBM[[#This Row],[Avg_Upmove]]="", "", tbl_IBM[[#This Row],[Avg_Upmove]]/tbl_IBM[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0900-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="63">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0900-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="107">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9060,47 +9060,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="tbl_ORCL" displayName="tbl_ORCL" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="202"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Open" totalsRowDxfId="62" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="High" totalsRowDxfId="61" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Low" totalsRowDxfId="60" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Close" totalsRowDxfId="59" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Adj Close" totalsRowDxfId="58" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Open" totalsRowDxfId="105" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="High" totalsRowDxfId="104" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Low" totalsRowDxfId="103" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Close" totalsRowDxfId="102" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="Adj Close" totalsRowDxfId="101" dataCellStyle="Currency"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0A00-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="EMA" dataDxfId="201" totalsRowDxfId="57" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0A00-000008000000}" name="EMA" dataDxfId="100" totalsRowDxfId="99" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_ORCL[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="RSI" dataDxfId="200" totalsRowDxfId="56" dataCellStyle="Currency">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0A00-000009000000}" name="RSI" dataDxfId="98" totalsRowDxfId="97" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_ORCL[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_ORCL[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="BB_Mean" dataDxfId="199" totalsRowDxfId="55" dataCellStyle="Currency">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0A00-00000A000000}" name="BB_Mean" dataDxfId="96" totalsRowDxfId="95" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="BB_Upper" dataDxfId="198" totalsRowDxfId="54" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0A00-00000B000000}" name="BB_Upper" dataDxfId="94" totalsRowDxfId="93" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_ORCL[[#This Row],[BB_Mean]]="", "", tbl_ORCL[[#This Row],[BB_Mean]]+(BB_Width*tbl_ORCL[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="BB_Lower" dataDxfId="197" totalsRowDxfId="53" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0A00-00000C000000}" name="BB_Lower" dataDxfId="92" totalsRowDxfId="91" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_ORCL[[#This Row],[BB_Mean]]="", "", tbl_ORCL[[#This Row],[BB_Mean]]-(BB_Width*tbl_ORCL[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0A00-00000D000000}" name="Move" dataDxfId="196" totalsRowDxfId="52" dataCellStyle="Currency">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0A00-00000D000000}" name="Move" dataDxfId="90" totalsRowDxfId="89" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW(tbl_ORCL[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0A00-00000E000000}" name="Upmove" dataDxfId="195" totalsRowDxfId="51" dataCellStyle="Currency">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0A00-00000E000000}" name="Upmove" dataDxfId="88" totalsRowDxfId="87" dataCellStyle="Currency">
       <calculatedColumnFormula>MAX(tbl_ORCL[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0A00-00000F000000}" name="Downmove" dataDxfId="194" totalsRowDxfId="50" dataCellStyle="Currency">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0A00-00000F000000}" name="Downmove" dataDxfId="86" totalsRowDxfId="85" dataCellStyle="Currency">
       <calculatedColumnFormula>MAX(-tbl_ORCL[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0A00-000010000000}" name="Avg_Upmove" dataDxfId="193" totalsRowDxfId="49" dataCellStyle="Currency">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0A00-000010000000}" name="Avg_Upmove" dataDxfId="84" totalsRowDxfId="83" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0A00-000011000000}" name="Avg_Downmove" dataDxfId="192" totalsRowDxfId="48" dataCellStyle="Currency">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0A00-000011000000}" name="Avg_Downmove" dataDxfId="82" totalsRowDxfId="81" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0A00-000012000000}" name="RS" dataDxfId="191" totalsRowDxfId="47" dataCellStyle="Currency">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0A00-000012000000}" name="RS" dataDxfId="80" totalsRowDxfId="79" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_ORCL[[#This Row],[Avg_Upmove]]="", "", tbl_ORCL[[#This Row],[Avg_Upmove]]/tbl_ORCL[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0A00-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="190" totalsRowDxfId="46" dataCellStyle="Currency">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0A00-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="78" totalsRowDxfId="77" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9112,47 +9112,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="tbl_AKRO" displayName="tbl_AKRO" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Open" totalsRowDxfId="45" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="High" totalsRowDxfId="44" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Low" totalsRowDxfId="43" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Close" totalsRowDxfId="42" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="Adj Close" totalsRowDxfId="41" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Open" totalsRowDxfId="75" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="High" totalsRowDxfId="74" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Low" totalsRowDxfId="73" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Close" totalsRowDxfId="72" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="Adj Close" totalsRowDxfId="71" dataCellStyle="Currency"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0B00-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="EMA" totalsRowDxfId="40" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0B00-000008000000}" name="EMA" totalsRowDxfId="70" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_AKRO[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0B00-000009000000}" name="RSI" dataDxfId="188">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0B00-000009000000}" name="RSI" dataDxfId="69">
       <calculatedColumnFormula>IF(tbl_AKRO[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_AKRO[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0B00-00000A000000}" name="BB_Mean" totalsRowDxfId="39" dataCellStyle="Currency">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0B00-00000A000000}" name="BB_Mean" totalsRowDxfId="68" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0B00-00000B000000}" name="BB_Upper" dataDxfId="187" totalsRowDxfId="38" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0B00-00000B000000}" name="BB_Upper" dataDxfId="67" totalsRowDxfId="66" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_AKRO[[#This Row],[BB_Mean]]="", "", tbl_AKRO[[#This Row],[BB_Mean]]+(BB_Width*tbl_AKRO[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0B00-00000C000000}" name="BB_Lower" dataDxfId="186" totalsRowDxfId="37" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0B00-00000C000000}" name="BB_Lower" dataDxfId="65" totalsRowDxfId="64" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_AKRO[[#This Row],[BB_Mean]]="", "", tbl_AKRO[[#This Row],[BB_Mean]]-(BB_Width*tbl_AKRO[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0B00-00000D000000}" name="Move" dataDxfId="185">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0B00-00000D000000}" name="Move" dataDxfId="63">
       <calculatedColumnFormula>IF(ROW(tbl_AKRO[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0B00-00000E000000}" name="Upmove" dataDxfId="184">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0B00-00000E000000}" name="Upmove" dataDxfId="62">
       <calculatedColumnFormula>MAX(tbl_AKRO[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0B00-00000F000000}" name="Downmove" dataDxfId="183">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0B00-00000F000000}" name="Downmove" dataDxfId="61">
       <calculatedColumnFormula>MAX(-tbl_AKRO[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0B00-000010000000}" name="Avg_Upmove" dataDxfId="182">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0B00-000010000000}" name="Avg_Upmove" dataDxfId="60">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0B00-000011000000}" name="Avg_Downmove" dataDxfId="181">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0B00-000011000000}" name="Avg_Downmove" dataDxfId="59">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0B00-000012000000}" name="RS" dataDxfId="180">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0B00-000012000000}" name="RS" dataDxfId="58">
       <calculatedColumnFormula>IF(tbl_AKRO[[#This Row],[Avg_Upmove]]="", "", tbl_AKRO[[#This Row],[Avg_Upmove]]/tbl_AKRO[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0B00-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="36" dataCellStyle="Currency">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0B00-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="57" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9164,47 +9164,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="tbl_FDX" displayName="tbl_FDX" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Open" totalsRowDxfId="26" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="High" totalsRowDxfId="25" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Low" totalsRowDxfId="24" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Close" totalsRowDxfId="23" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Adj Close" totalsRowDxfId="22" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Open" totalsRowDxfId="55" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="High" totalsRowDxfId="54" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Low" totalsRowDxfId="53" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Close" totalsRowDxfId="52" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0C00-000006000000}" name="Adj Close" totalsRowDxfId="51" dataCellStyle="Currency"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0C00-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="EMA" totalsRowDxfId="21" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0C00-000008000000}" name="EMA" totalsRowDxfId="50" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_FDX[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="RSI" dataDxfId="34">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0C00-000009000000}" name="RSI" dataDxfId="49">
       <calculatedColumnFormula>IF(tbl_FDX[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_FDX[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="BB_Mean" totalsRowDxfId="20" dataCellStyle="Currency">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0C00-00000A000000}" name="BB_Mean" totalsRowDxfId="48" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0C00-00000B000000}" name="BB_Upper" totalsRowDxfId="19" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0C00-00000B000000}" name="BB_Upper" totalsRowDxfId="47" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_FDX[[#This Row],[BB_Mean]]="", "", tbl_FDX[[#This Row],[BB_Mean]]+(BB_Width*tbl_FDX[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0C00-00000C000000}" name="BB_Lower" dataDxfId="33" totalsRowDxfId="18" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0C00-00000C000000}" name="BB_Lower" dataDxfId="46" totalsRowDxfId="45" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_FDX[[#This Row],[BB_Mean]]="", "", tbl_FDX[[#This Row],[BB_Mean]]-(BB_Width*tbl_FDX[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0C00-00000D000000}" name="Move" dataDxfId="32">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0C00-00000D000000}" name="Move" dataDxfId="44">
       <calculatedColumnFormula>IF(ROW(tbl_FDX[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0C00-00000E000000}" name="Upmove" dataDxfId="31">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0C00-00000E000000}" name="Upmove" dataDxfId="43">
       <calculatedColumnFormula>MAX(tbl_FDX[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0C00-00000F000000}" name="Downmove" dataDxfId="30">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0C00-00000F000000}" name="Downmove" dataDxfId="42">
       <calculatedColumnFormula>MAX(-tbl_FDX[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0C00-000010000000}" name="Avg_Upmove" dataDxfId="29">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0C00-000010000000}" name="Avg_Upmove" dataDxfId="41">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0C00-000011000000}" name="Avg_Downmove" dataDxfId="28">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0C00-000011000000}" name="Avg_Downmove" dataDxfId="40">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0C00-000012000000}" name="RS" dataDxfId="27">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0C00-000012000000}" name="RS" dataDxfId="39">
       <calculatedColumnFormula>IF(tbl_FDX[[#This Row],[Avg_Upmove]]="", "", tbl_FDX[[#This Row],[Avg_Upmove]]/tbl_FDX[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0C00-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="17" dataCellStyle="Currency">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0C00-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="38" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9216,47 +9216,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="tbl_NKLA" displayName="tbl_NKLA" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="37"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Open"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="High"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="Low"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Close"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0D00-000006000000}" name="Adj Close"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0D00-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="EMA" totalsRowDxfId="4" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0D00-000008000000}" name="EMA" totalsRowDxfId="36" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_NKLA[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="RSI" dataDxfId="178">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0D00-000009000000}" name="RSI" dataDxfId="35">
       <calculatedColumnFormula>IF(tbl_NKLA[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_NKLA[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0D00-00000A000000}" name="BB_Mean" totalsRowDxfId="3" dataCellStyle="Currency">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0D00-00000A000000}" name="BB_Mean" totalsRowDxfId="34" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0D00-00000B000000}" name="BB_Upper" totalsRowDxfId="2" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0D00-00000B000000}" name="BB_Upper" totalsRowDxfId="33" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_NKLA[[#This Row],[BB_Mean]]="", "", tbl_NKLA[[#This Row],[BB_Mean]]+(BB_Width*tbl_NKLA[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0D00-00000C000000}" name="BB_Lower" totalsRowDxfId="1" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0D00-00000C000000}" name="BB_Lower" totalsRowDxfId="32" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_NKLA[[#This Row],[BB_Mean]]="", "", tbl_NKLA[[#This Row],[BB_Mean]]-(BB_Width*tbl_NKLA[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0D00-00000D000000}" name="Move" dataDxfId="177">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0D00-00000D000000}" name="Move" dataDxfId="31">
       <calculatedColumnFormula>IF(ROW(tbl_NKLA[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0D00-00000E000000}" name="Upmove" dataDxfId="176">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0D00-00000E000000}" name="Upmove" dataDxfId="30">
       <calculatedColumnFormula>MAX(tbl_NKLA[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0D00-00000F000000}" name="Downmove" dataDxfId="175">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0D00-00000F000000}" name="Downmove" dataDxfId="29">
       <calculatedColumnFormula>MAX(-tbl_NKLA[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0D00-000010000000}" name="Avg_Upmove" dataDxfId="174">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0D00-000010000000}" name="Avg_Upmove" dataDxfId="28">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0D00-000011000000}" name="Avg_Downmove" dataDxfId="173">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0D00-000011000000}" name="Avg_Downmove" dataDxfId="27">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0D00-000012000000}" name="RS" dataDxfId="172">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0D00-000012000000}" name="RS" dataDxfId="26">
       <calculatedColumnFormula>IF(tbl_NKLA[[#This Row],[Avg_Upmove]]="", "", tbl_NKLA[[#This Row],[Avg_Upmove]]/tbl_NKLA[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0D00-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0D00-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="25" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9268,44 +9268,44 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="tbl_SPXS" displayName="tbl_SPXS" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-000012000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="171"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Open" totalsRowDxfId="16" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="High" totalsRowDxfId="15" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="Low" totalsRowDxfId="14" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Close" totalsRowDxfId="13" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="Adj Close" totalsRowDxfId="12" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="Open" totalsRowDxfId="23" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="High" totalsRowDxfId="22" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="Low" totalsRowDxfId="21" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0E00-000005000000}" name="Close" totalsRowDxfId="20" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0E00-000006000000}" name="Adj Close" totalsRowDxfId="19" dataCellStyle="Currency"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0E00-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="EMA" totalsRowDxfId="11" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0E00-000008000000}" name="EMA" totalsRowDxfId="18" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_SPXS[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="RSI" dataDxfId="170">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0E00-000009000000}" name="RSI" dataDxfId="17">
       <calculatedColumnFormula>IF(tbl_SPXS[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_SPXS[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0E00-00000A000000}" name="BB_Mean" totalsRowDxfId="10" dataCellStyle="Currency">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0E00-00000A000000}" name="BB_Mean" totalsRowDxfId="16" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0E00-00000B000000}" name="BB_Upper" totalsRowDxfId="9" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0E00-00000B000000}" name="BB_Upper" totalsRowDxfId="15" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_SPXS[[#This Row],[BB_Mean]]="", "", tbl_SPXS[[#This Row],[BB_Mean]]+(BB_Width*tbl_SPXS[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0E00-00000C000000}" name="BB_Lower" totalsRowDxfId="8" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0E00-00000C000000}" name="BB_Lower" totalsRowDxfId="14" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_SPXS[[#This Row],[BB_Mean]]="", "", tbl_SPXS[[#This Row],[BB_Mean]]-(BB_Width*tbl_SPXS[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0E00-00000D000000}" name="Move" dataDxfId="169">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0E00-00000D000000}" name="Move" dataDxfId="13">
       <calculatedColumnFormula>IF(ROW(tbl_SPXS[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0E00-00000E000000}" name="Upmove" dataDxfId="168">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0E00-00000E000000}" name="Upmove" dataDxfId="12">
       <calculatedColumnFormula>MAX(tbl_SPXS[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0E00-00000F000000}" name="Downmove" dataDxfId="167">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0E00-00000F000000}" name="Downmove" dataDxfId="11">
       <calculatedColumnFormula>MAX(-tbl_SPXS[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0E00-000010000000}" name="Avg_Upmove" dataDxfId="166">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0E00-000010000000}" name="Avg_Upmove" dataDxfId="10">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0E00-000011000000}" name="Avg_Downmove" dataDxfId="165">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0E00-000011000000}" name="Avg_Downmove" dataDxfId="9">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0E00-000012000000}" name="RS" dataDxfId="164">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0E00-000012000000}" name="RS" dataDxfId="8">
       <calculatedColumnFormula>IF(tbl_SPXS[[#This Row],[Avg_Upmove]]="", "", tbl_SPXS[[#This Row],[Avg_Upmove]]/tbl_SPXS[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0E00-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="7" dataCellStyle="Currency">
@@ -9330,7 +9330,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="# Holdings">
       <calculatedColumnFormula>INDEX(tbl_position[], COUNT(tbl_position[Date]), MATCH("Shares_"&amp;C5, pos_header,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="Total" totalsRowFunction="sum" dataDxfId="163">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="Total" totalsRowFunction="sum" dataDxfId="6">
       <calculatedColumnFormula>tbl_holdings[[#This Row],[Current Price]]*tbl_holdings[[#This Row],['# Holdings]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9343,22 +9343,22 @@
   <autoFilter ref="J4:P10" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1000-000001000000}" name="Index"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Start" dataDxfId="162">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1000-000002000000}" name="Start" dataDxfId="5">
       <calculatedColumnFormula>K4+7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="End" dataDxfId="161">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1000-000003000000}" name="End" dataDxfId="4">
       <calculatedColumnFormula>L4+7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="BUY" dataDxfId="160">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1000-000004000000}" name="BUY" dataDxfId="3">
       <calculatedColumnFormula>ABS(SUMIFS(tbl_transaction[Net_Cash_Change], tbl_transaction[Transactions], M$4, tbl_transaction[Transaction_Date], "&gt;="&amp;tbl_transsummary[[#This Row],[Start]], tbl_transaction[Transaction_Date], "&lt;=" &amp;tbl_transsummary[[#This Row],[End]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="SELL" dataDxfId="159">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1000-000005000000}" name="SELL" dataDxfId="2">
       <calculatedColumnFormula>ABS(SUMIFS(tbl_transaction[Net_Cash_Change], tbl_transaction[Transactions], N$4, tbl_transaction[Transaction_Date], "&gt;="&amp;tbl_transsummary[[#This Row],[Start]], tbl_transaction[Transaction_Date], "&lt;=" &amp;tbl_transsummary[[#This Row],[End]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="SHORT" dataDxfId="158">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1000-000006000000}" name="SHORT" dataDxfId="1">
       <calculatedColumnFormula>ABS(SUMIFS(tbl_transaction[Net_Stock_Change], tbl_transaction[Transactions], O$4, tbl_transaction[Transaction_Date], "&gt;="&amp;tbl_transsummary[[#This Row],[Start]], tbl_transaction[Transaction_Date], "&lt;=" &amp;tbl_transsummary[[#This Row],[End]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="COVER" dataDxfId="157">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-1000-000007000000}" name="COVER" dataDxfId="0">
       <calculatedColumnFormula>ABS(SUMIFS(tbl_transaction[Net_Stock_Change], tbl_transaction[Transactions], P$4, tbl_transaction[Transaction_Date], "&gt;="&amp;tbl_transsummary[[#This Row],[Start]], tbl_transaction[Transaction_Date], "&lt;=" &amp;tbl_transsummary[[#This Row],[End]]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9367,7 +9367,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tbl_symbol" displayName="tbl_symbol" ref="A3:A13" totalsRowShown="0" headerRowDxfId="254">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tbl_symbol" displayName="tbl_symbol" ref="A3:A13" totalsRowShown="0" headerRowDxfId="238">
   <autoFilter ref="A3:A13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Symbol"/>
@@ -9377,7 +9377,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tbl_transtype" displayName="tbl_transtype" ref="C3:C7" totalsRowShown="0" headerRowDxfId="253">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tbl_transtype" displayName="tbl_transtype" ref="C3:C7" totalsRowShown="0" headerRowDxfId="237">
   <autoFilter ref="C3:C7" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Transactions"/>
@@ -9387,7 +9387,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tbl_Metrics" displayName="tbl_Metrics" ref="E3:E6" totalsRowShown="0" headerRowDxfId="252">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tbl_Metrics" displayName="tbl_Metrics" ref="E3:E6" totalsRowShown="0" headerRowDxfId="236">
   <autoFilter ref="E3:E6" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Metrics"/>
@@ -9400,77 +9400,77 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="tbl_position" displayName="tbl_position" ref="A4:Y23" totalsRowCount="1">
   <autoFilter ref="A4:Y22" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="25">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="140"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="235"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Price_AAPL" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_AAPL[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Price_RIOT" dataDxfId="139" dataCellStyle="Currency">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Price_RIOT" dataDxfId="234" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_RIOT[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Price_HD" totalsRowDxfId="6" dataCellStyle="Currency">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Price_HD" totalsRowDxfId="233" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_HD[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Price_WMT" dataDxfId="138" dataCellStyle="Currency">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Price_WMT" dataDxfId="232" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_WMT[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Price_IBM" dataDxfId="137" dataCellStyle="Currency">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Price_IBM" dataDxfId="231" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_IBM[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Price_ORCL" dataDxfId="136" dataCellStyle="Currency">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0400-000007000000}" name="Price_ORCL" dataDxfId="230" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_ORCL[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0400-000014000000}" name="Price_AKRO" dataDxfId="135" dataCellStyle="Currency">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0400-000014000000}" name="Price_AKRO" dataDxfId="229" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_AKRO[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0400-000013000000}" name="Price_FDX" dataDxfId="134" dataCellStyle="Currency">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0400-000013000000}" name="Price_FDX" dataDxfId="228" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_FDX[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0400-000015000000}" name="Price_NKLA" dataDxfId="133" dataCellStyle="Currency">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0400-000015000000}" name="Price_NKLA" dataDxfId="227" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_NKLA[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0400-000016000000}" name="Price_SPXS" dataDxfId="132" dataCellStyle="Currency">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0400-000016000000}" name="Price_SPXS" dataDxfId="226" dataCellStyle="Currency">
       <calculatedColumnFormula>VLOOKUP(tbl_position[[#This Row],[Date]], tbl_SPXS[], 5, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Shares_AAPL" dataDxfId="131">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0400-000008000000}" name="Shares_AAPL" dataDxfId="225">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_AAPL]], FIND("_", tbl_position[[#Headers],[Shares_AAPL]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $L4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Shares_RIOT" dataDxfId="130">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0400-000009000000}" name="Shares_RIOT" dataDxfId="224">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_RIOT]], FIND("_", tbl_position[[#Headers],[Shares_RIOT]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $M4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Shares_HD" dataDxfId="129">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0400-00000A000000}" name="Shares_HD" dataDxfId="223">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_HD]], FIND("_", tbl_position[[#Headers],[Shares_HD]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $N4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Shares_WMT" dataDxfId="128">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0400-00000B000000}" name="Shares_WMT" dataDxfId="222">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_WMT]], FIND("_", tbl_position[[#Headers],[Shares_WMT]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $O4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="Shares_IBM" dataDxfId="127">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0400-00000C000000}" name="Shares_IBM" dataDxfId="221">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_IBM]], FIND("_", tbl_position[[#Headers],[Shares_IBM]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $P4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="Shares_ORCL" dataDxfId="126">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0400-00000D000000}" name="Shares_ORCL" dataDxfId="220">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_ORCL]], FIND("_", tbl_position[[#Headers],[Shares_ORCL]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $Q4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0400-00001A000000}" name="Shares_AKRO" dataDxfId="125">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0400-00001A000000}" name="Shares_AKRO" dataDxfId="219">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_AKRO]], FIND("_", tbl_position[[#Headers],[Shares_AKRO]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $R4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0400-000019000000}" name="Shares_FDX" dataDxfId="124">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0400-000019000000}" name="Shares_FDX" dataDxfId="218">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_FDX]], FIND("_", tbl_position[[#Headers],[Shares_FDX]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $S4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0400-000018000000}" name="Shares_NKLA" dataDxfId="123">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0400-000018000000}" name="Shares_NKLA" dataDxfId="217">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_NKLA]], FIND("_", tbl_position[[#Headers],[Shares_NKLA]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $T4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0400-000017000000}" name="Shares_SPXS" dataDxfId="122">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0400-000017000000}" name="Shares_SPXS" dataDxfId="216">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Stock Holding Change], tbl_transaction[Symbol], MID(tbl_position[[#Headers],[Shares_SPXS]], FIND("_", tbl_position[[#Headers],[Shares_SPXS]])+1, 99), tbl_transaction[Transaction_Date], tbl_position[[#This Row],[Date]]) + IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $U4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0400-00000E000000}" name="Shares_Holding" dataCellStyle="Currency">
       <calculatedColumnFormula xml:space="preserve"> SUMPRODUCT(INDIRECT(ADDRESS(ROW(V5), 2)):INDIRECT(ADDRESS(ROW(V5), MATCH("Shares_AAPL", pos_header,0)-1)), INDIRECT(ADDRESS(ROW(V5), MATCH("Shares_AAPL", pos_header,0))): INDIRECT(ADDRESS(ROW(V5), MATCH("Shares_Holding", pos_header,0)-1)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="Cash_Holding" dataDxfId="121" totalsRowDxfId="5" dataCellStyle="Currency">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0400-00000F000000}" name="Cash_Holding" dataDxfId="215" totalsRowDxfId="214" dataCellStyle="Currency">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Net_Cash_Change], tbl_transaction[Transaction_Date],tbl_position[[#This Row],[Date]])+IF(tbl_position[[#This Row],[Date]]=$A$5, 100000, $W4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="Liabilities_Holding" dataDxfId="120">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0400-000010000000}" name="Liabilities_Holding" dataDxfId="213">
       <calculatedColumnFormula>SUMIFS(tbl_transaction[Net_Debt_Change], tbl_transaction[Transaction_Date],tbl_position[[#This Row],[Date]])+IF(tbl_position[[#This Row],[Date]]=$A$5, 0, $X4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="Total_Net_Asset" dataDxfId="119">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0400-000012000000}" name="Total_Net_Asset" dataDxfId="212">
       <calculatedColumnFormula>tbl_position[[#This Row],[Shares_Holding]]+tbl_position[[#This Row],[Cash_Holding]]-tbl_position[[#This Row],[Liabilities_Holding]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9482,47 +9482,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="tbl_HD" displayName="tbl_HD" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Open" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="High" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Low" dataDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Close" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Adj Close" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="211"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Open" dataDxfId="210"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="High" dataDxfId="209"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Low" dataDxfId="208"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Close" dataDxfId="207"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Adj Close" dataDxfId="206"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="EMA" totalsRowDxfId="103" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="EMA" totalsRowDxfId="205" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_HD[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="RSI" dataDxfId="112">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="RSI" dataDxfId="204">
       <calculatedColumnFormula>IF(tbl_HD[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_HD[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="BB_Mean" totalsRowDxfId="102" dataCellStyle="Currency">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="BB_Mean" totalsRowDxfId="203" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="BB_Upper" dataDxfId="111" totalsRowDxfId="101" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="BB_Upper" dataDxfId="202" totalsRowDxfId="201" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_HD[[#This Row],[BB_Mean]]="", "", tbl_HD[[#This Row],[BB_Mean]]+(BB_Width*tbl_HD[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="BB_Lower" dataDxfId="110" totalsRowDxfId="100" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="BB_Lower" dataDxfId="200" totalsRowDxfId="199" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_HD[[#This Row],[BB_Mean]]="", "", tbl_HD[[#This Row],[BB_Mean]]-(BB_Width*tbl_HD[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Move" dataDxfId="109">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Move" dataDxfId="198">
       <calculatedColumnFormula>IF(ROW(tbl_HD[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="Upmove" dataDxfId="108">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0500-00000E000000}" name="Upmove" dataDxfId="197">
       <calculatedColumnFormula>MAX(tbl_HD[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Downmove" dataDxfId="107">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Downmove" dataDxfId="196">
       <calculatedColumnFormula>MAX(-tbl_HD[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Avg_Upmove" dataDxfId="106">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Avg_Upmove" dataDxfId="195">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Avg_Downmove" dataDxfId="105">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Avg_Downmove" dataDxfId="194">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="RS" dataDxfId="104">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0500-000012000000}" name="RS" dataDxfId="193">
       <calculatedColumnFormula>IF(tbl_HD[[#This Row],[Avg_Upmove]]="", "", tbl_HD[[#This Row],[Avg_Upmove]]/tbl_HD[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0500-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="99" dataCellStyle="Currency">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0500-000013000000}" name="BB_Stdev" totalsRowFunction="count" totalsRowDxfId="192" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9534,47 +9534,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="tbl_AAPL" displayName="tbl_AAPL" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="251"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Open" totalsRowDxfId="98" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="High" totalsRowDxfId="97" dataCellStyle="Currency"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Low" totalsRowDxfId="96" dataCellStyle="Currency"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Close" totalsRowDxfId="95" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Adj Close" totalsRowDxfId="94" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="191"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Open" totalsRowDxfId="190" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="High" totalsRowDxfId="189" dataCellStyle="Currency"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Low" totalsRowDxfId="188" dataCellStyle="Currency"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Close" totalsRowDxfId="187" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Adj Close" totalsRowDxfId="186" dataCellStyle="Currency"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="EMA" dataDxfId="250" totalsRowDxfId="93" dataCellStyle="Currency">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="EMA" dataDxfId="185" totalsRowDxfId="184" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_AAPL[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="RSI" dataDxfId="249" totalsRowDxfId="92" dataCellStyle="Currency">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="RSI" dataDxfId="183" totalsRowDxfId="182" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_AAPL[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_AAPL[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="BB_Mean" dataDxfId="248" totalsRowDxfId="91" dataCellStyle="Currency">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="BB_Mean" dataDxfId="181" totalsRowDxfId="180" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="BB_Upper" dataDxfId="247" totalsRowDxfId="90" dataCellStyle="Currency">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="BB_Upper" dataDxfId="179" totalsRowDxfId="178" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_AAPL[[#This Row],[BB_Mean]]="", "", tbl_AAPL[[#This Row],[BB_Mean]]+(BB_Width*tbl_AAPL[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="BB_Lower" dataDxfId="246" totalsRowDxfId="89" dataCellStyle="Currency">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="BB_Lower" dataDxfId="177" totalsRowDxfId="176" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_AAPL[[#This Row],[BB_Mean]]="", "", tbl_AAPL[[#This Row],[BB_Mean]]-(BB_Width*tbl_AAPL[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Move" dataDxfId="245" totalsRowDxfId="88" dataCellStyle="Currency">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Move" dataDxfId="175" totalsRowDxfId="174" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW(tbl_AAPL[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Upmove" dataDxfId="244" totalsRowDxfId="87" dataCellStyle="Currency">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Upmove" dataDxfId="173" totalsRowDxfId="172" dataCellStyle="Currency">
       <calculatedColumnFormula>MAX(tbl_AAPL[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Downmove" dataDxfId="243" totalsRowDxfId="86" dataCellStyle="Currency">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Downmove" dataDxfId="171" totalsRowDxfId="170" dataCellStyle="Currency">
       <calculatedColumnFormula>MAX(-tbl_AAPL[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Avg_Upmove" dataDxfId="242" totalsRowDxfId="85" dataCellStyle="Currency">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Avg_Upmove" dataDxfId="169" totalsRowDxfId="168" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0600-000011000000}" name="Avg_Downmove" dataDxfId="241" totalsRowDxfId="84" dataCellStyle="Currency">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0600-000011000000}" name="Avg_Downmove" dataDxfId="167" totalsRowDxfId="166" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0600-000012000000}" name="RS" dataDxfId="240" totalsRowDxfId="83" dataCellStyle="Currency">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0600-000012000000}" name="RS" dataDxfId="165" totalsRowDxfId="164" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_AAPL[[#This Row],[Avg_Upmove]]="", "", tbl_AAPL[[#This Row],[Avg_Upmove]]/tbl_AAPL[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0600-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="239" totalsRowDxfId="82" dataCellStyle="Currency">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0600-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="163" totalsRowDxfId="162" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9586,47 +9586,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="tbl_WMT" displayName="tbl_WMT" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="238"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Open" dataDxfId="237"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="High" dataDxfId="236"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Low" dataDxfId="235"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Close" dataDxfId="234"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Adj Close" dataDxfId="233"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="161"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Open" dataDxfId="160"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="High" dataDxfId="159"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Low" dataDxfId="158"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Close" dataDxfId="157"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Adj Close" dataDxfId="156"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="EMA" dataDxfId="232">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="EMA" dataDxfId="155">
       <calculatedColumnFormula>IF(tbl_WMT[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="RSI" dataDxfId="231" totalsRowDxfId="81" dataCellStyle="Currency">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="RSI" dataDxfId="154" totalsRowDxfId="153" dataCellStyle="Currency">
       <calculatedColumnFormula>IF(tbl_WMT[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_WMT[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="BB_Mean" dataDxfId="230">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="BB_Mean" dataDxfId="152">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="BB_Upper" dataDxfId="229">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="BB_Upper" dataDxfId="151">
       <calculatedColumnFormula>IF(tbl_WMT[[#This Row],[BB_Mean]]="", "", tbl_WMT[[#This Row],[BB_Mean]]+(BB_Width*tbl_WMT[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="BB_Lower" dataDxfId="228">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="BB_Lower" dataDxfId="150">
       <calculatedColumnFormula>IF(tbl_WMT[[#This Row],[BB_Mean]]="", "", tbl_WMT[[#This Row],[BB_Mean]]-(BB_Width*tbl_WMT[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Move" dataDxfId="227">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Move" dataDxfId="149">
       <calculatedColumnFormula>IF(ROW(tbl_WMT[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="Upmove" dataDxfId="226">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0700-00000E000000}" name="Upmove" dataDxfId="148">
       <calculatedColumnFormula>MAX(tbl_WMT[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Downmove" dataDxfId="225">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0700-00000F000000}" name="Downmove" dataDxfId="147">
       <calculatedColumnFormula>MAX(-tbl_WMT[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Avg_Upmove" dataDxfId="224">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0700-000010000000}" name="Avg_Upmove" dataDxfId="146">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Avg_Downmove" dataDxfId="223">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0700-000011000000}" name="Avg_Downmove" dataDxfId="145">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="RS" dataDxfId="222">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0700-000012000000}" name="RS" dataDxfId="144">
       <calculatedColumnFormula>IF(tbl_WMT[[#This Row],[Avg_Upmove]]="", "", tbl_WMT[[#This Row],[Avg_Upmove]]/tbl_WMT[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0700-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="221">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0700-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="143">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9638,47 +9638,47 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="tbl_RIOT" displayName="tbl_RIOT" ref="A4:S45" totalsRowCount="1">
   <autoFilter ref="A4:S44" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="220"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Open" dataDxfId="219"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="High" dataDxfId="218"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Low" dataDxfId="217"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Close" dataDxfId="216"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Adj Close" dataDxfId="215"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Date" totalsRowLabel="Total" dataDxfId="142"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Open" dataDxfId="141"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="High" dataDxfId="140"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Low" dataDxfId="139"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Close" dataDxfId="138"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="Adj Close" dataDxfId="137"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0800-000007000000}" name="Volume"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="EMA" dataDxfId="214">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0800-000008000000}" name="EMA" dataDxfId="136">
       <calculatedColumnFormula>IF(tbl_RIOT[[#This Row],[Date]]=$A$5, $F5, EMA_Beta*$H4 + (1-EMA_Beta)*$F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="RSI" dataDxfId="213">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0800-000009000000}" name="RSI" dataDxfId="135">
       <calculatedColumnFormula>IF(tbl_RIOT[[#This Row],[RS]]= "", "", 100-(100/(1+tbl_RIOT[[#This Row],[RS]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="BB_Mean" dataDxfId="212">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0800-00000A000000}" name="BB_Mean" dataDxfId="134">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="BB_Upper" dataDxfId="211">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0800-00000B000000}" name="BB_Upper" dataDxfId="133">
       <calculatedColumnFormula>IF(tbl_RIOT[[#This Row],[BB_Mean]]="", "", tbl_RIOT[[#This Row],[BB_Mean]]+(BB_Width*tbl_RIOT[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="BB_Lower" dataDxfId="210">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0800-00000C000000}" name="BB_Lower" dataDxfId="132">
       <calculatedColumnFormula>IF(tbl_RIOT[[#This Row],[BB_Mean]]="", "", tbl_RIOT[[#This Row],[BB_Mean]]-(BB_Width*tbl_RIOT[[#This Row],[BB_Stdev]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="Move" dataDxfId="209">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0800-00000D000000}" name="Move" dataDxfId="131">
       <calculatedColumnFormula>IF(ROW(tbl_RIOT[[#This Row],[Adj Close]])=5, 0, $F5-$F4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="Upmove" dataDxfId="208">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0800-00000E000000}" name="Upmove" dataDxfId="130">
       <calculatedColumnFormula>MAX(tbl_RIOT[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Downmove" dataDxfId="207">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0800-00000F000000}" name="Downmove" dataDxfId="129">
       <calculatedColumnFormula>MAX(-tbl_RIOT[[#This Row],[Move]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Avg_Upmove" dataDxfId="206">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0800-000010000000}" name="Avg_Upmove" dataDxfId="128">
       <calculatedColumnFormula>IF(ROW($N5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($N5)-RSI_Periods +1, MATCH("Upmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($N5),MATCH("Upmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Avg_Downmove" dataDxfId="205">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0800-000011000000}" name="Avg_Downmove" dataDxfId="127">
       <calculatedColumnFormula>IF(ROW($O5)-5&lt;RSI_Periods, "", AVERAGE(INDIRECT(ADDRESS(ROW($O5)-RSI_Periods +1, MATCH("Downmove", Price_Header,0))): INDIRECT(ADDRESS(ROW($O5),MATCH("Downmove", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="RS" dataDxfId="204">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0800-000012000000}" name="RS" dataDxfId="126">
       <calculatedColumnFormula>IF(tbl_RIOT[[#This Row],[Avg_Upmove]]="", "", tbl_RIOT[[#This Row],[Avg_Upmove]]/tbl_RIOT[[#This Row],[Avg_Downmove]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0800-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="203">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0800-000013000000}" name="BB_Stdev" totalsRowFunction="count" dataDxfId="125">
       <calculatedColumnFormula>IF(ROW($N5)-4&lt;BB_Periods, "", _xlfn.STDEV.S(INDIRECT(ADDRESS(ROW($F5)-RSI_Periods +1, MATCH("Adj Close", Price_Header,0))): INDIRECT(ADDRESS(ROW($F5),MATCH("Adj Close", Price_Header,0)))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -28605,8 +28605,8 @@
   </sheetPr>
   <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView topLeftCell="F21" zoomScale="95" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="95" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -28684,8 +28684,8 @@
         <v>195</v>
       </c>
       <c r="G3" s="89">
-        <f>DATE(2020, 9, 25)</f>
-        <v>44099</v>
+        <f>DATE(2020, 10, 5)</f>
+        <v>44109</v>
       </c>
       <c r="H3" s="68"/>
       <c r="I3" s="85"/>
@@ -28905,7 +28905,7 @@
       </c>
       <c r="G10" s="109">
         <f>INDEX(tbl_transsummary[], _xlfn.FLOOR.MATH(($G$3-DATE(2020, 9, 9))/7)+1, 4)</f>
-        <v>12305</v>
+        <v>0</v>
       </c>
       <c r="H10" s="71"/>
       <c r="I10" s="85"/>
@@ -28943,7 +28943,7 @@
       </c>
       <c r="G11" s="113">
         <f>INDEX(tbl_transsummary[], _xlfn.FLOOR.MATH(($G$3-DATE(2020, 9, 9))/7)+1, 5)</f>
-        <v>11844.4</v>
+        <v>0</v>
       </c>
       <c r="H11" s="68"/>
       <c r="I11" s="85"/>
@@ -28981,7 +28981,7 @@
       </c>
       <c r="G12" s="111">
         <f>INDEX(tbl_transsummary[], _xlfn.FLOOR.MATH(($G$3-DATE(2020, 9, 9))/7)+1, 6)</f>
-        <v>15616</v>
+        <v>0</v>
       </c>
       <c r="H12" s="68"/>
       <c r="I12" s="85"/>
@@ -31854,7 +31854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>

</xml_diff>